<commit_message>
added layer-related proba and correlation processing
</commit_message>
<xml_diff>
--- a/data/performances.xlsx
+++ b/data/performances.xlsx
@@ -5,21 +5,23 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Vincent\Videos\Better Call Saul\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Eclipse\workspaces\Networks\TopicControl\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10920"/>
   </bookViews>
   <sheets>
-    <sheet name="performances" sheetId="1" r:id="rId1"/>
+    <sheet name="properties" sheetId="3" r:id="rId1"/>
+    <sheet name="raw" sheetId="1" r:id="rId2"/>
+    <sheet name="normalized" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="63">
   <si>
     <t>CKM_Physicians_Innovation/</t>
   </si>
@@ -45,6 +47,81 @@
     <t>Vickers_Chan_7thGraders/</t>
   </si>
   <si>
+    <t>a=0.01;b=0.01</t>
+  </si>
+  <si>
+    <t>a=0.1;b=0.01</t>
+  </si>
+  <si>
+    <t>a=0.5;b=0.01</t>
+  </si>
+  <si>
+    <t>a=0.8;b=0.01</t>
+  </si>
+  <si>
+    <t>a=0.99;b=0.01</t>
+  </si>
+  <si>
+    <t>a=0.01;b=0.1</t>
+  </si>
+  <si>
+    <t>a=0.1;b=0.1</t>
+  </si>
+  <si>
+    <t>a=0.5;b=0.1</t>
+  </si>
+  <si>
+    <t>a=0.8;b=0.1</t>
+  </si>
+  <si>
+    <t>a=0.99;b=0.1</t>
+  </si>
+  <si>
+    <t>a=0.01;b=0.5</t>
+  </si>
+  <si>
+    <t>a=0.1;b=0.5</t>
+  </si>
+  <si>
+    <t>a=0.5;b=0.5</t>
+  </si>
+  <si>
+    <t>a=0.8;b=0.5</t>
+  </si>
+  <si>
+    <t>a=0.99;b=0.5</t>
+  </si>
+  <si>
+    <t>a=0.01;b=0.8</t>
+  </si>
+  <si>
+    <t>a=0.1;b=0.8</t>
+  </si>
+  <si>
+    <t>a=0.5;b=0.8</t>
+  </si>
+  <si>
+    <t>a=0.8;b=0.8</t>
+  </si>
+  <si>
+    <t>a=0.99;b=0.8</t>
+  </si>
+  <si>
+    <t>a=0.01;b=0.99</t>
+  </si>
+  <si>
+    <t>a=0.1;b=0.99</t>
+  </si>
+  <si>
+    <t>a=0.5;b=0.99</t>
+  </si>
+  <si>
+    <t>a=0.8;b=0.99</t>
+  </si>
+  <si>
+    <t>a=0.99;b=0.99</t>
+  </si>
+  <si>
     <t>a=0,01;b=0,01</t>
   </si>
   <si>
@@ -118,12 +195,30 @@
   </si>
   <si>
     <t>a=0,99;b=0,99</t>
+  </si>
+  <si>
+    <t>Nodes</t>
+  </si>
+  <si>
+    <t>Links</t>
+  </si>
+  <si>
+    <t>LinkTypes</t>
+  </si>
+  <si>
+    <t>AverageDistance</t>
+  </si>
+  <si>
+    <t>Density</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.000"/>
+  </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -441,7 +536,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -556,6 +651,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -601,10 +705,16 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -926,31 +1036,463 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="26.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.21875" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4">
+        <v>246</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1551</v>
+      </c>
+      <c r="D2" s="4">
+        <v>3</v>
+      </c>
+      <c r="E2" s="4">
+        <v>480</v>
+      </c>
+      <c r="F2" s="7">
+        <v>7.9641612742658002E-3</v>
+      </c>
+      <c r="G2" s="5">
+        <v>3.481095564156</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E3">
+        <v>565</v>
+      </c>
+      <c r="F3" s="8">
+        <v>9.3744814999170405E-3</v>
+      </c>
+      <c r="G3" s="1">
+        <v>4.5041479668162703</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E4">
+        <v>506</v>
+      </c>
+      <c r="F4" s="8">
+        <v>8.39555334328854E-3</v>
+      </c>
+      <c r="G4" s="1">
+        <v>3.6691050963179701</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="4">
+        <v>61</v>
+      </c>
+      <c r="C5" s="4">
+        <v>620</v>
+      </c>
+      <c r="D5" s="4">
+        <v>5</v>
+      </c>
+      <c r="E5" s="4">
+        <v>193</v>
+      </c>
+      <c r="F5" s="7">
+        <v>0.10546448087431699</v>
+      </c>
+      <c r="G5" s="5">
+        <v>3.1887005649717501</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E6">
+        <v>124</v>
+      </c>
+      <c r="F6" s="8">
+        <v>6.7759562841529994E-2</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1.9556451612903201</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E7">
+        <v>21</v>
+      </c>
+      <c r="F7" s="8">
+        <v>1.1475409836065599E-2</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E8">
+        <v>88</v>
+      </c>
+      <c r="F8" s="8">
+        <v>4.8087431693989102E-2</v>
+      </c>
+      <c r="G8" s="1">
+        <v>3.1159114857744998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E9">
+        <v>194</v>
+      </c>
+      <c r="F9" s="8">
+        <v>0.106010928961749</v>
+      </c>
+      <c r="G9" s="1">
+        <v>2.3903954802259899</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="4">
+        <v>39</v>
+      </c>
+      <c r="C10" s="4">
+        <v>1018</v>
+      </c>
+      <c r="D10" s="4">
+        <v>4</v>
+      </c>
+      <c r="E10" s="4">
+        <v>316</v>
+      </c>
+      <c r="F10" s="7">
+        <v>0.213225371120108</v>
+      </c>
+      <c r="G10" s="5">
+        <v>2.0431848852901502</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E11">
+        <v>446</v>
+      </c>
+      <c r="F11" s="8">
+        <v>0.30094466936572201</v>
+      </c>
+      <c r="G11" s="1">
+        <v>1.7719298245613999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E12">
+        <v>109</v>
+      </c>
+      <c r="F12" s="8">
+        <v>7.3549257759784104E-2</v>
+      </c>
+      <c r="G12" s="1">
+        <v>3.2889105058365802</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E13">
+        <v>147</v>
+      </c>
+      <c r="F13" s="8">
+        <v>9.9190283400809695E-2</v>
+      </c>
+      <c r="G13" s="1">
+        <v>2.7194388777555099</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="4">
+        <v>21</v>
+      </c>
+      <c r="C14" s="4">
+        <v>312</v>
+      </c>
+      <c r="D14" s="4">
+        <v>3</v>
+      </c>
+      <c r="E14" s="4">
+        <v>190</v>
+      </c>
+      <c r="F14" s="7">
+        <v>0.452380952380952</v>
+      </c>
+      <c r="G14" s="5">
+        <v>1.64047619047619</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E15">
+        <v>102</v>
+      </c>
+      <c r="F15" s="8">
+        <v>0.24285714285714299</v>
+      </c>
+      <c r="G15" s="1">
+        <v>2.1026315789473702</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E16">
+        <v>20</v>
+      </c>
+      <c r="F16" s="8">
+        <v>4.7619047619047603E-2</v>
+      </c>
+      <c r="G16" s="1">
+        <v>1.44444444444444</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="4">
+        <v>71</v>
+      </c>
+      <c r="C17" s="4">
+        <v>2223</v>
+      </c>
+      <c r="D17" s="4">
+        <v>3</v>
+      </c>
+      <c r="E17" s="4">
+        <v>612</v>
+      </c>
+      <c r="F17" s="7">
+        <v>0.123138832997988</v>
+      </c>
+      <c r="G17" s="5">
+        <v>2.33844121532365</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E18">
+        <v>855</v>
+      </c>
+      <c r="F18" s="8">
+        <v>0.17203219315895399</v>
+      </c>
+      <c r="G18" s="1">
+        <v>2.11571103291244</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E19">
+        <v>756</v>
+      </c>
+      <c r="F19" s="8">
+        <v>0.15211267605633799</v>
+      </c>
+      <c r="G19" s="1">
+        <v>2.1035196687370599</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="4">
+        <v>369</v>
+      </c>
+      <c r="C20" s="4">
+        <v>441</v>
+      </c>
+      <c r="D20" s="4">
+        <v>3</v>
+      </c>
+      <c r="E20" s="4">
+        <v>312</v>
+      </c>
+      <c r="F20" s="7">
+        <v>4.5952633439377902E-3</v>
+      </c>
+      <c r="G20" s="5">
+        <v>13.9633182998497</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E21">
+        <v>83</v>
+      </c>
+      <c r="F21" s="8">
+        <v>1.2224578767526799E-3</v>
+      </c>
+      <c r="G21" s="1">
+        <v>13.4857478695269</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E22">
+        <v>46</v>
+      </c>
+      <c r="F22" s="8">
+        <v>6.77506775067751E-4</v>
+      </c>
+      <c r="G22" s="1">
+        <v>8.23232323232323</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="4">
+        <v>16</v>
+      </c>
+      <c r="C23" s="4">
+        <v>35</v>
+      </c>
+      <c r="D23" s="4">
+        <v>2</v>
+      </c>
+      <c r="E23" s="4">
+        <v>20</v>
+      </c>
+      <c r="F23" s="7">
+        <v>0.16666666666666699</v>
+      </c>
+      <c r="G23" s="5">
+        <v>2.4857142857142902</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E24">
+        <v>15</v>
+      </c>
+      <c r="F24" s="8">
+        <v>0.125</v>
+      </c>
+      <c r="G24" s="1">
+        <v>2.3818181818181801</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="4">
+        <v>29</v>
+      </c>
+      <c r="C25" s="4">
+        <v>740</v>
+      </c>
+      <c r="D25" s="4">
+        <v>3</v>
+      </c>
+      <c r="E25" s="4">
+        <v>361</v>
+      </c>
+      <c r="F25" s="7">
+        <v>0.44458128078817699</v>
+      </c>
+      <c r="G25" s="5">
+        <v>1.6256157635468</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E26">
+        <v>181</v>
+      </c>
+      <c r="F26" s="8">
+        <v>0.22290640394088701</v>
+      </c>
+      <c r="G26" s="1">
+        <v>2.79433497536946</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E27">
+        <v>198</v>
+      </c>
+      <c r="F27" s="8">
+        <v>0.24384236453201999</v>
+      </c>
+      <c r="G27" s="1">
+        <v>2.10582010582011</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="3"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="20" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="25" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="18" max="20" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="23" max="25" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
         <v>8</v>
       </c>
@@ -1027,648 +1569,1395 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>127.461557790694</v>
+        <v>548.96126760271795</v>
       </c>
       <c r="C2" s="1">
-        <v>127.256052084419</v>
+        <v>546.99720524522002</v>
       </c>
       <c r="D2" s="1">
-        <v>126.463003658896</v>
+        <v>538.46801880582098</v>
       </c>
       <c r="E2" s="1">
-        <v>125.975358701655</v>
+        <v>532.28539282689496</v>
       </c>
       <c r="F2" s="1">
-        <v>125.710834330298</v>
+        <v>528.46472001402196</v>
       </c>
       <c r="G2" s="1">
-        <v>127.459827005359</v>
+        <v>548.93935388057196</v>
       </c>
       <c r="H2" s="1">
-        <v>127.24009621635901</v>
+        <v>546.77999639843995</v>
       </c>
       <c r="I2" s="1">
-        <v>126.394183803705</v>
+        <v>537.42482734203497</v>
       </c>
       <c r="J2" s="1">
-        <v>125.888925025014</v>
+        <v>530.66770980898696</v>
       </c>
       <c r="K2" s="1">
-        <v>125.61341042844199</v>
+        <v>526.50314030966399</v>
       </c>
       <c r="L2" s="1">
-        <v>127.44261365407399</v>
+        <v>548.74660111672802</v>
       </c>
       <c r="M2" s="1">
-        <v>127.08439307958599</v>
+        <v>544.87735764888498</v>
       </c>
       <c r="N2" s="1">
-        <v>125.872840196632</v>
+        <v>528.46472001402196</v>
       </c>
       <c r="O2" s="1">
-        <v>125.203902785236</v>
+        <v>516.99524178787601</v>
       </c>
       <c r="P2" s="1">
-        <v>124.855106815376</v>
+        <v>510.10363891131601</v>
       </c>
       <c r="Q2" s="1">
-        <v>127.37991602608599</v>
+        <v>548.097227205423</v>
       </c>
       <c r="R2" s="1">
-        <v>126.609170600609</v>
+        <v>538.57261853581201</v>
       </c>
       <c r="S2" s="1">
-        <v>124.644925205143</v>
+        <v>501.141024448655</v>
       </c>
       <c r="T2" s="1">
-        <v>124.135795565367</v>
+        <v>478.31732888328901</v>
       </c>
       <c r="U2" s="1">
-        <v>124.03503659248101</v>
+        <v>466.18982169188899</v>
       </c>
       <c r="V2" s="1">
-        <v>126.008099804735</v>
+        <v>528.46472001402299</v>
       </c>
       <c r="W2" s="1">
-        <v>124.82469764321399</v>
+        <v>428.25977331500002</v>
       </c>
       <c r="X2" s="1">
-        <v>148.03408269184999</v>
+        <v>378.73293453914499</v>
       </c>
       <c r="Y2" s="1">
-        <v>175.330188899712</v>
+        <v>392.22518602022899</v>
       </c>
       <c r="Z2" s="1">
-        <v>195.65747634961099</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+        <v>406.261125697154</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>887.98530498171795</v>
+        <v>1410.2365781655601</v>
       </c>
       <c r="C3" s="1">
-        <v>884.03050068273603</v>
+        <v>1407.75519110205</v>
       </c>
       <c r="D3" s="1">
-        <v>866.65357325964203</v>
+        <v>1396.9267839613401</v>
       </c>
       <c r="E3" s="1">
-        <v>853.835142591313</v>
+        <v>1389.01974268606</v>
       </c>
       <c r="F3" s="1">
-        <v>845.811793939925</v>
+        <v>1384.1069402872899</v>
       </c>
       <c r="G3" s="1">
-        <v>887.94125768643505</v>
+        <v>1410.20897413578</v>
       </c>
       <c r="H3" s="1">
-        <v>883.591961522411</v>
+        <v>1407.4810803646899</v>
       </c>
       <c r="I3" s="1">
-        <v>864.50385062453995</v>
+        <v>1395.5991093960199</v>
       </c>
       <c r="J3" s="1">
-        <v>850.44715417498799</v>
+        <v>1386.9469183272899</v>
       </c>
       <c r="K3" s="1">
-        <v>841.65957453784495</v>
+        <v>1381.58214795704</v>
       </c>
       <c r="L3" s="1">
-        <v>887.55125852642595</v>
+        <v>1409.96548195126</v>
       </c>
       <c r="M3" s="1">
-        <v>879.71730895754899</v>
+        <v>1405.07114541603</v>
       </c>
       <c r="N3" s="1">
-        <v>845.69367747204899</v>
+        <v>1384.10469901846</v>
       </c>
       <c r="O3" s="1">
-        <v>821.02658473715201</v>
+        <v>1369.2221789620601</v>
       </c>
       <c r="P3" s="1">
-        <v>805.78120569484497</v>
+        <v>1360.17000912854</v>
       </c>
       <c r="Q3" s="1">
-        <v>886.22924502275498</v>
+        <v>1409.14297580532</v>
       </c>
       <c r="R3" s="1">
-        <v>866.69323832460304</v>
+        <v>1397.03661176077</v>
       </c>
       <c r="S3" s="1">
-        <v>784.93031105718399</v>
+        <v>1348.1659819460001</v>
       </c>
       <c r="T3" s="1">
-        <v>729.03358257320895</v>
+        <v>1316.4876598691801</v>
       </c>
       <c r="U3" s="1">
-        <v>696.03761155520897</v>
+        <v>1297.7552444289099</v>
       </c>
       <c r="V3" s="1">
-        <v>845.27911139205003</v>
+        <v>1384.0202357107701</v>
       </c>
       <c r="W3" s="1">
-        <v>551.67911369180194</v>
+        <v>1212.7261597827101</v>
       </c>
       <c r="X3" s="1">
-        <v>338.21772797489098</v>
+        <v>968.63834490633099</v>
       </c>
       <c r="Y3" s="1">
-        <v>345.40191846413302</v>
+        <v>954.32725054400896</v>
       </c>
       <c r="Z3" s="1">
-        <v>359.96031889842999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+        <v>962.07017534023498</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>4653.7576247398301</v>
+        <v>1250.0509612011799</v>
       </c>
       <c r="C4" s="1">
-        <v>4647.5647065864296</v>
+        <v>1247.9048313288199</v>
       </c>
       <c r="D4" s="1">
-        <v>4620.2406059127597</v>
+        <v>1238.5664570630699</v>
       </c>
       <c r="E4" s="1">
-        <v>4599.9617947018896</v>
+        <v>1231.7632742728399</v>
       </c>
       <c r="F4" s="1">
-        <v>4587.2135381055195</v>
+        <v>1227.50809171537</v>
       </c>
       <c r="G4" s="1">
-        <v>4653.68873724484</v>
+        <v>1250.02776943759</v>
       </c>
       <c r="H4" s="1">
-        <v>4646.87776230902</v>
+        <v>1247.6748484038101</v>
       </c>
       <c r="I4" s="1">
-        <v>4616.8487883584303</v>
+        <v>1237.4595360114799</v>
       </c>
       <c r="J4" s="1">
-        <v>4594.5863712142</v>
+        <v>1230.02204814074</v>
       </c>
       <c r="K4" s="1">
-        <v>4580.6018025941503</v>
+        <v>1225.3705790665199</v>
       </c>
       <c r="L4" s="1">
-        <v>4653.0807523529602</v>
+        <v>1249.8227004181599</v>
       </c>
       <c r="M4" s="1">
-        <v>4640.8229953070404</v>
+        <v>1245.64961629086</v>
       </c>
       <c r="N4" s="1">
-        <v>4587.1323292737598</v>
+        <v>1227.7886232743199</v>
       </c>
       <c r="O4" s="1">
-        <v>4547.7088877890201</v>
+        <v>1214.86265448414</v>
       </c>
       <c r="P4" s="1">
-        <v>4523.1151289131903</v>
+        <v>1206.84484618806</v>
       </c>
       <c r="Q4" s="1">
-        <v>4651.0245992291302</v>
+        <v>1249.1284476819201</v>
       </c>
       <c r="R4" s="1">
-        <v>4620.4535303128396</v>
+        <v>1238.90535314917</v>
       </c>
       <c r="S4" s="1">
-        <v>4489.5531430621604</v>
+        <v>1196.2464224375501</v>
       </c>
       <c r="T4" s="1">
-        <v>4396.70395636167</v>
+        <v>1166.1921208988799</v>
       </c>
       <c r="U4" s="1">
-        <v>4340.260710775</v>
+        <v>1147.9681290706001</v>
       </c>
       <c r="V4" s="1">
-        <v>4586.8120226813899</v>
+        <v>1227.9399804452</v>
       </c>
       <c r="W4" s="1">
-        <v>4070.1574159607599</v>
+        <v>1062.49418874916</v>
       </c>
       <c r="X4" s="1">
-        <v>2925.8054745777899</v>
+        <v>807.66585753450397</v>
       </c>
       <c r="Y4" s="1">
-        <v>2789.3318264610398</v>
+        <v>819.63680536070501</v>
       </c>
       <c r="Z4" s="1">
-        <v>2795.8489398177499</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+        <v>848.81765861107101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="1">
-        <v>46.5364796523547</v>
+        <v>1662.67085446228</v>
       </c>
       <c r="C5" s="1">
-        <v>46.117277099905799</v>
+        <v>1658.2581667229799</v>
       </c>
       <c r="D5" s="1">
-        <v>44.454134569219498</v>
+        <v>1638.84620080891</v>
       </c>
       <c r="E5" s="1">
-        <v>43.389382410414001</v>
+        <v>1624.50149022398</v>
       </c>
       <c r="F5" s="1">
-        <v>42.7497867409908</v>
+        <v>1615.5114971606299</v>
       </c>
       <c r="G5" s="1">
-        <v>46.531798506222202</v>
+        <v>1662.62173379146</v>
       </c>
       <c r="H5" s="1">
-        <v>46.072395841786403</v>
+        <v>1657.76888838934</v>
       </c>
       <c r="I5" s="1">
-        <v>44.272621683185598</v>
+        <v>1636.4426619107901</v>
       </c>
       <c r="J5" s="1">
-        <v>43.125196502938799</v>
+        <v>1620.70725131113</v>
       </c>
       <c r="K5" s="1">
-        <v>42.437835974567001</v>
+        <v>1610.8564295363001</v>
       </c>
       <c r="L5" s="1">
-        <v>46.490674533319499</v>
+        <v>1662.18955987917</v>
       </c>
       <c r="M5" s="1">
-        <v>45.686195645051903</v>
+        <v>1653.47203815535</v>
       </c>
       <c r="N5" s="1">
-        <v>42.799236270286201</v>
+        <v>1615.5114971606399</v>
       </c>
       <c r="O5" s="1">
-        <v>41.015527589787901</v>
+        <v>1587.8810914146</v>
       </c>
       <c r="P5" s="1">
-        <v>40.010522718620301</v>
+        <v>1570.7542344421099</v>
       </c>
       <c r="Q5" s="1">
-        <v>46.353051247248303</v>
+        <v>1660.73213959186</v>
       </c>
       <c r="R5" s="1">
-        <v>44.501306620366897</v>
+        <v>1639.08683528233</v>
       </c>
       <c r="S5" s="1">
-        <v>38.921271338752</v>
+        <v>1547.78548279554</v>
       </c>
       <c r="T5" s="1">
-        <v>36.537730710316801</v>
+        <v>1484.5594684304399</v>
       </c>
       <c r="U5" s="1">
-        <v>35.727618995699402</v>
+        <v>1446.8438259992199</v>
       </c>
       <c r="V5" s="1">
-        <v>42.836666978679297</v>
+        <v>1615.5114971606399</v>
       </c>
       <c r="W5" s="1">
-        <v>36.432414641028501</v>
+        <v>1274.98200857147</v>
       </c>
       <c r="X5" s="1">
-        <v>128.39170472603001</v>
+        <v>772.77372350590099</v>
       </c>
       <c r="Y5" s="1">
-        <v>264.76653207211501</v>
+        <v>812.65205630232003</v>
       </c>
       <c r="Z5" s="1">
-        <v>379.42697522229798</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+        <v>875.91361967236105</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1">
-        <v>789.941815466462</v>
+        <v>7513.1887612104401</v>
       </c>
       <c r="C6" s="1">
-        <v>788.03923197149095</v>
+        <v>7506.6587495578897</v>
       </c>
       <c r="D6" s="1">
-        <v>779.78328517447096</v>
+        <v>7477.8364553003103</v>
       </c>
       <c r="E6" s="1">
-        <v>773.79955586083895</v>
+        <v>7456.4339986288996</v>
       </c>
       <c r="F6" s="1">
-        <v>770.06917364421804</v>
+        <v>7442.9740997866502</v>
       </c>
       <c r="G6" s="1">
-        <v>789.92067683482401</v>
+        <v>7513.1161253556402</v>
       </c>
       <c r="H6" s="1">
-        <v>787.82977543134996</v>
+        <v>7505.93432027366</v>
       </c>
       <c r="I6" s="1">
-        <v>778.77888639016601</v>
+        <v>7474.2571814088597</v>
       </c>
       <c r="J6" s="1">
-        <v>772.23303284764495</v>
+        <v>7450.7586074383198</v>
       </c>
       <c r="K6" s="1">
-        <v>768.15184250287905</v>
+        <v>7435.9911248025901</v>
       </c>
       <c r="L6" s="1">
-        <v>789.73484751547699</v>
+        <v>7512.4763670778302</v>
       </c>
       <c r="M6" s="1">
-        <v>785.99648686648004</v>
+        <v>7499.5617021896196</v>
       </c>
       <c r="N6" s="1">
-        <v>770.129273310342</v>
+        <v>7442.9488619684498</v>
       </c>
       <c r="O6" s="1">
-        <v>758.75315453058101</v>
+        <v>7401.3310215093898</v>
       </c>
       <c r="P6" s="1">
-        <v>751.73543595607498</v>
+        <v>7375.3462493220404</v>
       </c>
       <c r="Q6" s="1">
-        <v>789.10938123277901</v>
+        <v>7510.3164385814398</v>
       </c>
       <c r="R6" s="1">
-        <v>779.93263089438506</v>
+        <v>7478.1526365481104</v>
       </c>
       <c r="S6" s="1">
-        <v>742.50144774930595</v>
+        <v>7340.1104513475102</v>
       </c>
       <c r="T6" s="1">
-        <v>717.10800920468103</v>
+        <v>7240.4383800586602</v>
       </c>
       <c r="U6" s="1">
-        <v>702.205467268593</v>
+        <v>7178.4812493135896</v>
       </c>
       <c r="V6" s="1">
-        <v>770.21456716400905</v>
+        <v>7442.8392842702096</v>
       </c>
       <c r="W6" s="1">
-        <v>639.06790100164301</v>
+        <v>6864.1897822593801</v>
       </c>
       <c r="X6" s="1">
-        <v>572.46080728003005</v>
+        <v>5282.7019321481503</v>
       </c>
       <c r="Y6" s="1">
-        <v>618.11254066717095</v>
+        <v>5087.2696176652098</v>
       </c>
       <c r="Z6" s="1">
-        <v>658.51552555022397</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+        <v>5103.7521672045204</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="1">
-        <v>369.14038892815</v>
+        <v>161.11196439222499</v>
       </c>
       <c r="C7" s="1">
-        <v>367.74785723886498</v>
+        <v>160.987556889525</v>
       </c>
       <c r="D7" s="1">
-        <v>361.75880710261498</v>
+        <v>160.60094070829001</v>
       </c>
       <c r="E7" s="1">
-        <v>357.48128335105997</v>
+        <v>160.39161221417999</v>
       </c>
       <c r="F7" s="1">
-        <v>354.86717528218401</v>
+        <v>160.278184663009</v>
       </c>
       <c r="G7" s="1">
-        <v>369.12482554676399</v>
+        <v>161.11049127957901</v>
       </c>
       <c r="H7" s="1">
-        <v>367.59415179965799</v>
+        <v>160.97475413772</v>
       </c>
       <c r="I7" s="1">
-        <v>361.03313267672399</v>
+        <v>160.565190670193</v>
       </c>
       <c r="J7" s="1">
-        <v>356.37162759378299</v>
+        <v>160.34714415255999</v>
       </c>
       <c r="K7" s="1">
-        <v>353.53427931285802</v>
+        <v>160.229985770464</v>
       </c>
       <c r="L7" s="1">
-        <v>368.98795578158899</v>
+        <v>161.09761587931499</v>
       </c>
       <c r="M7" s="1">
-        <v>366.25034303680201</v>
+        <v>160.87088902396999</v>
       </c>
       <c r="N7" s="1">
-        <v>354.867175282186</v>
+        <v>160.30269558547201</v>
       </c>
       <c r="O7" s="1">
-        <v>347.16979946622098</v>
+        <v>160.04812064406201</v>
       </c>
       <c r="P7" s="1">
-        <v>342.66719478277997</v>
+        <v>159.933578255849</v>
       </c>
       <c r="Q7" s="1">
-        <v>368.52718699079099</v>
+        <v>161.05532807009001</v>
       </c>
       <c r="R7" s="1">
-        <v>361.83165512881902</v>
+        <v>160.60947399321199</v>
       </c>
       <c r="S7" s="1">
-        <v>336.97373574227902</v>
+        <v>159.863312629506</v>
       </c>
       <c r="T7" s="1">
-        <v>323.31979588154701</v>
+        <v>159.771812661914</v>
       </c>
       <c r="U7" s="1">
-        <v>316.02782061824502</v>
+        <v>159.828203480734</v>
       </c>
       <c r="V7" s="1">
-        <v>354.86717528218497</v>
+        <v>160.31035132549499</v>
       </c>
       <c r="W7" s="1">
-        <v>292.02358580844702</v>
+        <v>160.96174462529001</v>
       </c>
       <c r="X7" s="1">
-        <v>288.19577404889901</v>
+        <v>182.24163365358899</v>
       </c>
       <c r="Y7" s="1">
-        <v>305.809639189135</v>
+        <v>204.968105886861</v>
       </c>
       <c r="Z7" s="1">
-        <v>319.66606662517199</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+        <v>221.297315447762</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="1">
-        <v>12.826376296596401</v>
+        <v>114.762314698938</v>
       </c>
       <c r="C8" s="1">
-        <v>12.776638147592999</v>
+        <v>113.735474844751</v>
       </c>
       <c r="D8" s="1">
-        <v>12.6591601612182</v>
+        <v>109.371723130698</v>
       </c>
       <c r="E8" s="1">
-        <v>12.6431217508697</v>
+        <v>106.313174671466</v>
       </c>
       <c r="F8" s="1">
-        <v>12.6642413821539</v>
+        <v>104.47108494194801</v>
       </c>
       <c r="G8" s="1">
-        <v>12.8266007542386</v>
+        <v>114.75080284383699</v>
       </c>
       <c r="H8" s="1">
-        <v>12.780610527055201</v>
+        <v>113.622292275115</v>
       </c>
       <c r="I8" s="1">
-        <v>12.6784466569364</v>
+        <v>108.848832090795</v>
       </c>
       <c r="J8" s="1">
-        <v>12.6885043864027</v>
+        <v>105.528175177553</v>
       </c>
       <c r="K8" s="1">
-        <v>12.731930141162399</v>
+        <v>103.54011007891501</v>
       </c>
       <c r="L8" s="1">
-        <v>12.8257901651655</v>
+        <v>114.648152714731</v>
       </c>
       <c r="M8" s="1">
-        <v>12.790159467775201</v>
+        <v>112.621331216934</v>
       </c>
       <c r="N8" s="1">
-        <v>12.9543197505254</v>
+        <v>104.41158753055601</v>
       </c>
       <c r="O8" s="1">
-        <v>13.328806715928099</v>
+        <v>99.109656757970995</v>
       </c>
       <c r="P8" s="1">
-        <v>13.621524966150201</v>
+        <v>96.130984401875693</v>
       </c>
       <c r="Q8" s="1">
-        <v>12.816590752614401</v>
+        <v>114.298464014087</v>
       </c>
       <c r="R8" s="1">
-        <v>12.8505097318394</v>
+        <v>109.324535965753</v>
       </c>
       <c r="S8" s="1">
-        <v>14.5960723863422</v>
+        <v>92.374094724834293</v>
       </c>
       <c r="T8" s="1">
-        <v>16.599807435916901</v>
+        <v>85.185448409038599</v>
       </c>
       <c r="U8" s="1">
-        <v>18.074876675979901</v>
+        <v>82.915263726268194</v>
       </c>
       <c r="V8" s="1">
-        <v>13.1967967075734</v>
+        <v>104.187766531694</v>
       </c>
       <c r="W8" s="1">
-        <v>30.5688983214582</v>
+        <v>83.171464106190697</v>
       </c>
       <c r="X8" s="1">
-        <v>267.93236059517602</v>
+        <v>284.596373435857</v>
       </c>
       <c r="Y8" s="1">
-        <v>606.09908647117095</v>
+        <v>606.17621638538606</v>
       </c>
       <c r="Z8" s="1">
-        <v>891.04191243808305</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+        <v>880.86705519411998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1">
-        <v>2306.6224447354498</v>
+        <v>33.244391694526698</v>
       </c>
       <c r="C9" s="1">
-        <v>2301.0436447164898</v>
+        <v>32.8545973028031</v>
       </c>
       <c r="D9" s="1">
-        <v>2276.44895785054</v>
+        <v>31.322158111944301</v>
       </c>
       <c r="E9" s="1">
-        <v>2258.21720686356</v>
+        <v>30.380429146753599</v>
       </c>
       <c r="F9" s="1">
-        <v>2246.76542168384</v>
+        <v>29.842652236992901</v>
       </c>
       <c r="G9" s="1">
-        <v>2306.56045131784</v>
+        <v>33.2401233346461</v>
       </c>
       <c r="H9" s="1">
-        <v>2300.4256405278402</v>
+        <v>32.8138462404347</v>
       </c>
       <c r="I9" s="1">
-        <v>2273.4018255161</v>
+        <v>31.1613480542585</v>
       </c>
       <c r="J9" s="1">
-        <v>2253.3932614590199</v>
+        <v>30.161782306731101</v>
       </c>
       <c r="K9" s="1">
-        <v>2240.8361259823</v>
+        <v>29.5922606139519</v>
       </c>
       <c r="L9" s="1">
-        <v>2306.0134434922702</v>
+        <v>33.202630712138401</v>
       </c>
       <c r="M9" s="1">
-        <v>2294.9805850294001</v>
+        <v>32.464205709048102</v>
       </c>
       <c r="N9" s="1">
-        <v>2246.7326092960002</v>
+        <v>29.9254122625752</v>
       </c>
       <c r="O9" s="1">
-        <v>2211.3897890333301</v>
+        <v>28.546922197252499</v>
       </c>
       <c r="P9" s="1">
-        <v>2189.37980448189</v>
+        <v>27.869684722714101</v>
       </c>
       <c r="Q9" s="1">
-        <v>2304.1640757991599</v>
+        <v>33.077285779128196</v>
       </c>
       <c r="R9" s="1">
-        <v>2276.6779972269001</v>
+        <v>31.4070979259699</v>
       </c>
       <c r="S9" s="1">
-        <v>2159.4660953641401</v>
+        <v>27.486351188210399</v>
       </c>
       <c r="T9" s="1">
-        <v>2076.85907683921</v>
+        <v>26.709431773830801</v>
       </c>
       <c r="U9" s="1">
-        <v>2026.89181093006</v>
+        <v>26.7210593138545</v>
       </c>
       <c r="V9" s="1">
-        <v>2246.5044279574099</v>
+        <v>30.051171947187999</v>
       </c>
       <c r="W9" s="1">
-        <v>1791.2426497679301</v>
+        <v>31.670926807863498</v>
       </c>
       <c r="X9" s="1">
-        <v>1213.33160622949</v>
+        <v>123.566454342043</v>
       </c>
       <c r="Y9" s="1">
-        <v>1243.1843280451101</v>
+        <v>245.57026341033699</v>
       </c>
       <c r="Z9" s="1">
-        <v>1298.7374919748199</v>
+        <v>345.60749836986201</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Z9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="26.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="15" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="18" max="20" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="23" max="25" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>2.23154986830373</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2.22356587498057</v>
+      </c>
+      <c r="D2" s="1">
+        <v>2.1888943853895202</v>
+      </c>
+      <c r="E2" s="1">
+        <v>2.1637617594589198</v>
+      </c>
+      <c r="F2" s="1">
+        <v>2.1482305691626902</v>
+      </c>
+      <c r="G2" s="1">
+        <v>2.2314607881324098</v>
+      </c>
+      <c r="H2" s="1">
+        <v>2.2226829121887799</v>
+      </c>
+      <c r="I2" s="1">
+        <v>2.1846537696830701</v>
+      </c>
+      <c r="J2" s="1">
+        <v>2.1571858122316598</v>
+      </c>
+      <c r="K2" s="1">
+        <v>2.1402566679254602</v>
+      </c>
+      <c r="L2" s="1">
+        <v>2.2306772403119002</v>
+      </c>
+      <c r="M2" s="1">
+        <v>2.2149486083287999</v>
+      </c>
+      <c r="N2" s="1">
+        <v>2.1482305691626902</v>
+      </c>
+      <c r="O2" s="1">
+        <v>2.1016066739344499</v>
+      </c>
+      <c r="P2" s="1">
+        <v>2.0735920280947799</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>2.2280375089651301</v>
+      </c>
+      <c r="R2" s="1">
+        <v>2.1893195875439502</v>
+      </c>
+      <c r="S2" s="1">
+        <v>2.0371586359701399</v>
+      </c>
+      <c r="T2" s="1">
+        <v>1.94437938570443</v>
+      </c>
+      <c r="U2" s="1">
+        <v>1.89508057598329</v>
+      </c>
+      <c r="V2" s="1">
+        <v>2.1482305691626902</v>
+      </c>
+      <c r="W2" s="1">
+        <v>1.74089338745935</v>
+      </c>
+      <c r="X2" s="1">
+        <v>1.5395647745493699</v>
+      </c>
+      <c r="Y2" s="1">
+        <v>1.5944113252854799</v>
+      </c>
+      <c r="Z2" s="1">
+        <v>1.6514679906388401</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>23.118632428943599</v>
+      </c>
+      <c r="C3" s="1">
+        <v>23.077953952492599</v>
+      </c>
+      <c r="D3" s="1">
+        <v>22.900439081333499</v>
+      </c>
+      <c r="E3" s="1">
+        <v>22.770815453869801</v>
+      </c>
+      <c r="F3" s="1">
+        <v>22.6902777096278</v>
+      </c>
+      <c r="G3" s="1">
+        <v>23.118179903865201</v>
+      </c>
+      <c r="H3" s="1">
+        <v>23.0734603338474</v>
+      </c>
+      <c r="I3" s="1">
+        <v>22.8786739245249</v>
+      </c>
+      <c r="J3" s="1">
+        <v>22.7368347266768</v>
+      </c>
+      <c r="K3" s="1">
+        <v>22.648887671426898</v>
+      </c>
+      <c r="L3" s="1">
+        <v>23.114188228709299</v>
+      </c>
+      <c r="M3" s="1">
+        <v>23.0339532035415</v>
+      </c>
+      <c r="N3" s="1">
+        <v>22.690240967515699</v>
+      </c>
+      <c r="O3" s="1">
+        <v>22.4462652288863</v>
+      </c>
+      <c r="P3" s="1">
+        <v>22.297869002107198</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>23.100704521398701</v>
+      </c>
+      <c r="R3" s="1">
+        <v>22.9022395370617</v>
+      </c>
+      <c r="S3" s="1">
+        <v>22.1010816712459</v>
+      </c>
+      <c r="T3" s="1">
+        <v>21.581764915888201</v>
+      </c>
+      <c r="U3" s="1">
+        <v>21.274676138178901</v>
+      </c>
+      <c r="V3" s="1">
+        <v>22.6888563231273</v>
+      </c>
+      <c r="W3" s="1">
+        <v>19.8807567177493</v>
+      </c>
+      <c r="X3" s="1">
+        <v>15.879317129612</v>
+      </c>
+      <c r="Y3" s="1">
+        <v>15.644709025311601</v>
+      </c>
+      <c r="Z3" s="1">
+        <v>15.771642218692399</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
+        <v>32.0525887487481</v>
+      </c>
+      <c r="C4" s="1">
+        <v>31.997559777662001</v>
+      </c>
+      <c r="D4" s="1">
+        <v>31.758114283668402</v>
+      </c>
+      <c r="E4" s="1">
+        <v>31.583673699303699</v>
+      </c>
+      <c r="F4" s="1">
+        <v>31.474566454240101</v>
+      </c>
+      <c r="G4" s="1">
+        <v>32.051994088143502</v>
+      </c>
+      <c r="H4" s="1">
+        <v>31.9916627795848</v>
+      </c>
+      <c r="I4" s="1">
+        <v>31.729731692601899</v>
+      </c>
+      <c r="J4" s="1">
+        <v>31.539026875403501</v>
+      </c>
+      <c r="K4" s="1">
+        <v>31.4197584376032</v>
+      </c>
+      <c r="L4" s="1">
+        <v>32.046735908158098</v>
+      </c>
+      <c r="M4" s="1">
+        <v>31.939733751047601</v>
+      </c>
+      <c r="N4" s="1">
+        <v>31.481759571136401</v>
+      </c>
+      <c r="O4" s="1">
+        <v>31.150324473952299</v>
+      </c>
+      <c r="P4" s="1">
+        <v>30.9447396458478</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>32.028934555946698</v>
+      </c>
+      <c r="R4" s="1">
+        <v>31.766803926901702</v>
+      </c>
+      <c r="S4" s="1">
+        <v>30.672985190706399</v>
+      </c>
+      <c r="T4" s="1">
+        <v>29.902362074330199</v>
+      </c>
+      <c r="U4" s="1">
+        <v>29.435080232579399</v>
+      </c>
+      <c r="V4" s="1">
+        <v>31.485640524235802</v>
+      </c>
+      <c r="W4" s="1">
+        <v>27.243440737158</v>
+      </c>
+      <c r="X4" s="1">
+        <v>20.7093809624232</v>
+      </c>
+      <c r="Y4" s="1">
+        <v>21.016328342582199</v>
+      </c>
+      <c r="Z4" s="1">
+        <v>21.7645553490018</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <v>79.174802593441996</v>
+      </c>
+      <c r="C5" s="1">
+        <v>78.964674605856402</v>
+      </c>
+      <c r="D5" s="1">
+        <v>78.0402952766147</v>
+      </c>
+      <c r="E5" s="1">
+        <v>77.3572138201896</v>
+      </c>
+      <c r="F5" s="1">
+        <v>76.929118912411198</v>
+      </c>
+      <c r="G5" s="1">
+        <v>79.172463513878796</v>
+      </c>
+      <c r="H5" s="1">
+        <v>78.941375637587498</v>
+      </c>
+      <c r="I5" s="1">
+        <v>77.925841043370895</v>
+      </c>
+      <c r="J5" s="1">
+        <v>77.176535776720698</v>
+      </c>
+      <c r="K5" s="1">
+        <v>76.707449025537997</v>
+      </c>
+      <c r="L5" s="1">
+        <v>79.151883803769906</v>
+      </c>
+      <c r="M5" s="1">
+        <v>78.736763721683602</v>
+      </c>
+      <c r="N5" s="1">
+        <v>76.929118912411298</v>
+      </c>
+      <c r="O5" s="1">
+        <v>75.613385305457101</v>
+      </c>
+      <c r="P5" s="1">
+        <v>74.797820687719295</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>79.082482837707801</v>
+      </c>
+      <c r="R5" s="1">
+        <v>78.051754061063505</v>
+      </c>
+      <c r="S5" s="1">
+        <v>73.704070609311401</v>
+      </c>
+      <c r="T5" s="1">
+        <v>70.693308020497199</v>
+      </c>
+      <c r="U5" s="1">
+        <v>68.897325047581703</v>
+      </c>
+      <c r="V5" s="1">
+        <v>76.929118912411397</v>
+      </c>
+      <c r="W5" s="1">
+        <v>60.713428979593999</v>
+      </c>
+      <c r="X5" s="1">
+        <v>36.798748738376297</v>
+      </c>
+      <c r="Y5" s="1">
+        <v>38.697716966777101</v>
+      </c>
+      <c r="Z5" s="1">
+        <v>41.710172365350502</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1">
+        <v>105.819560017048</v>
+      </c>
+      <c r="C6" s="1">
+        <v>105.727588021942</v>
+      </c>
+      <c r="D6" s="1">
+        <v>105.321640215497</v>
+      </c>
+      <c r="E6" s="1">
+        <v>105.020197163787</v>
+      </c>
+      <c r="F6" s="1">
+        <v>104.830621123756</v>
+      </c>
+      <c r="G6" s="1">
+        <v>105.81853697683999</v>
+      </c>
+      <c r="H6" s="1">
+        <v>105.717384792587</v>
+      </c>
+      <c r="I6" s="1">
+        <v>105.271227907167</v>
+      </c>
+      <c r="J6" s="1">
+        <v>104.940262076596</v>
+      </c>
+      <c r="K6" s="1">
+        <v>104.732269363417</v>
+      </c>
+      <c r="L6" s="1">
+        <v>105.809526296871</v>
+      </c>
+      <c r="M6" s="1">
+        <v>105.62762960830401</v>
+      </c>
+      <c r="N6" s="1">
+        <v>104.83026566152699</v>
+      </c>
+      <c r="O6" s="1">
+        <v>104.24409889449799</v>
+      </c>
+      <c r="P6" s="1">
+        <v>103.87811618763401</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>105.779104768753</v>
+      </c>
+      <c r="R6" s="1">
+        <v>105.326093472509</v>
+      </c>
+      <c r="S6" s="1">
+        <v>103.38183734292301</v>
+      </c>
+      <c r="T6" s="1">
+        <v>101.97800535293899</v>
+      </c>
+      <c r="U6" s="1">
+        <v>101.105369708642</v>
+      </c>
+      <c r="V6" s="1">
+        <v>104.828722313665</v>
+      </c>
+      <c r="W6" s="1">
+        <v>96.678729327596898</v>
+      </c>
+      <c r="X6" s="1">
+        <v>74.404252565466905</v>
+      </c>
+      <c r="Y6" s="1">
+        <v>71.651684755847995</v>
+      </c>
+      <c r="Z6" s="1">
+        <v>71.883833340908694</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.43661778968082599</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.43628064197703398</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.435232901648481</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.43466561575658602</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.43435822401899499</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0.43661379750563301</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0.43624594617268397</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0.43513601807640501</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0.43454510610449898</v>
+      </c>
+      <c r="K7" s="1">
+        <v>0.43422760371399599</v>
+      </c>
+      <c r="L7" s="1">
+        <v>0.43657890482199102</v>
+      </c>
+      <c r="M7" s="1">
+        <v>0.43596446889964802</v>
+      </c>
+      <c r="N7" s="1">
+        <v>0.43442464928312302</v>
+      </c>
+      <c r="O7" s="1">
+        <v>0.43373474429285103</v>
+      </c>
+      <c r="P7" s="1">
+        <v>0.43342433131666402</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>0.436464303712982</v>
+      </c>
+      <c r="R7" s="1">
+        <v>0.435256027081876</v>
+      </c>
+      <c r="S7" s="1">
+        <v>0.43323390956505597</v>
+      </c>
+      <c r="T7" s="1">
+        <v>0.43298594217320702</v>
+      </c>
+      <c r="U7" s="1">
+        <v>0.43313876282041702</v>
+      </c>
+      <c r="V7" s="1">
+        <v>0.43444539654605602</v>
+      </c>
+      <c r="W7" s="1">
+        <v>0.43621069004143598</v>
+      </c>
+      <c r="X7" s="1">
+        <v>0.493879765998886</v>
+      </c>
+      <c r="Y7" s="1">
+        <v>0.55546912164461004</v>
+      </c>
+      <c r="Z7" s="1">
+        <v>0.59972172208065599</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1">
+        <v>7.1726446686836196</v>
+      </c>
+      <c r="C8" s="1">
+        <v>7.1084671777969497</v>
+      </c>
+      <c r="D8" s="1">
+        <v>6.8357326956686304</v>
+      </c>
+      <c r="E8" s="1">
+        <v>6.64457341696661</v>
+      </c>
+      <c r="F8" s="1">
+        <v>6.5294428088717602</v>
+      </c>
+      <c r="G8" s="1">
+        <v>7.1719251777398103</v>
+      </c>
+      <c r="H8" s="1">
+        <v>7.1013932671947</v>
+      </c>
+      <c r="I8" s="1">
+        <v>6.8030520056746902</v>
+      </c>
+      <c r="J8" s="1">
+        <v>6.59551094859704</v>
+      </c>
+      <c r="K8" s="1">
+        <v>6.4712568799321799</v>
+      </c>
+      <c r="L8" s="1">
+        <v>7.1655095446706802</v>
+      </c>
+      <c r="M8" s="1">
+        <v>7.0388332010583703</v>
+      </c>
+      <c r="N8" s="1">
+        <v>6.5257242206597299</v>
+      </c>
+      <c r="O8" s="1">
+        <v>6.1943535473731899</v>
+      </c>
+      <c r="P8" s="1">
+        <v>6.0081865251172299</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>7.1436540008804297</v>
+      </c>
+      <c r="R8" s="1">
+        <v>6.8327834978595501</v>
+      </c>
+      <c r="S8" s="1">
+        <v>5.7733809203021504</v>
+      </c>
+      <c r="T8" s="1">
+        <v>5.3240905255649098</v>
+      </c>
+      <c r="U8" s="1">
+        <v>5.1822039828917603</v>
+      </c>
+      <c r="V8" s="1">
+        <v>6.51173540823088</v>
+      </c>
+      <c r="W8" s="1">
+        <v>5.1982165066369204</v>
+      </c>
+      <c r="X8" s="1">
+        <v>17.787273339740999</v>
+      </c>
+      <c r="Y8" s="1">
+        <v>37.8860135240866</v>
+      </c>
+      <c r="Z8" s="1">
+        <v>55.054190949632499</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1.14635833429402</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1.13291714837252</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1.08007441765325</v>
+      </c>
+      <c r="E9" s="1">
+        <v>1.04760100506047</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1.02905697368941</v>
+      </c>
+      <c r="G9" s="1">
+        <v>1.14621114947056</v>
+      </c>
+      <c r="H9" s="1">
+        <v>1.1315119393253299</v>
+      </c>
+      <c r="I9" s="1">
+        <v>1.07452924325029</v>
+      </c>
+      <c r="J9" s="1">
+        <v>1.0400614588528001</v>
+      </c>
+      <c r="K9" s="1">
+        <v>1.02042277979145</v>
+      </c>
+      <c r="L9" s="1">
+        <v>1.1449183004185599</v>
+      </c>
+      <c r="M9" s="1">
+        <v>1.11945536927752</v>
+      </c>
+      <c r="N9" s="1">
+        <v>1.0319107676750101</v>
+      </c>
+      <c r="O9" s="1">
+        <v>0.98437662749146404</v>
+      </c>
+      <c r="P9" s="1">
+        <v>0.961023611128072</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>1.1405960613492501</v>
+      </c>
+      <c r="R9" s="1">
+        <v>1.08300337675758</v>
+      </c>
+      <c r="S9" s="1">
+        <v>0.94780521338656498</v>
+      </c>
+      <c r="T9" s="1">
+        <v>0.92101488875278603</v>
+      </c>
+      <c r="U9" s="1">
+        <v>0.92141583840877594</v>
+      </c>
+      <c r="V9" s="1">
+        <v>1.03624730852372</v>
+      </c>
+      <c r="W9" s="1">
+        <v>1.09210092440909</v>
+      </c>
+      <c r="X9" s="1">
+        <v>4.2609122186911303</v>
+      </c>
+      <c r="Y9" s="1">
+        <v>8.4679401175978199</v>
+      </c>
+      <c r="Z9" s="1">
+        <v>11.9174999437883</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>